<commit_message>
working script to plot sample locations
</commit_message>
<xml_diff>
--- a/data/sampling/metadata.xlsx
+++ b/data/sampling/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Liam/Desktop/UW/ECM/alhic1901_deep_layering/github/data/sampling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9405563-2F17-6748-997C-9F9EF3A0218E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D289C981-2B05-0743-A430-47105CE0987E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="760" windowWidth="29220" windowHeight="18880" xr2:uid="{A8C00553-77EA-744E-A26E-6C00C0051891}"/>
+    <workbookView xWindow="1040" yWindow="1740" windowWidth="29220" windowHeight="18880" xr2:uid="{A8C00553-77EA-744E-A26E-6C00C0051891}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>section</t>
   </si>
@@ -102,6 +102,42 @@
   </si>
   <si>
     <t>co2</t>
+  </si>
+  <si>
+    <t>meas_type</t>
+  </si>
+  <si>
+    <t>IC / CC</t>
+  </si>
+  <si>
+    <t>ICMPS</t>
+  </si>
+  <si>
+    <t>CO$_2$</t>
+  </si>
+  <si>
+    <t>CH$_4$</t>
+  </si>
+  <si>
+    <t>ISO</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>thin_section_vert</t>
+  </si>
+  <si>
+    <t>PP</t>
   </si>
 </sst>
 </file>
@@ -480,15 +516,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD79FB1-660A-A74C-AF5D-70A1289F30BA}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,326 +532,417 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1">
         <v>-110</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>-80</v>
       </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
       <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1">
         <v>50</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>80</v>
       </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
       <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1">
         <v>80</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>100</v>
       </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
       <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5">
         <v>-75</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>-40</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
       <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C6">
-        <v>0</v>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <v>50</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
       <c r="F6">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7">
         <v>-15</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>15</v>
       </c>
-      <c r="E7">
-        <v>-100</v>
-      </c>
       <c r="F7">
-        <v>-115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>-110</v>
+      </c>
+      <c r="G7">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8">
         <v>-110</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>-120</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
       <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9">
         <v>120</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>100</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
       <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10">
         <v>103</v>
       </c>
-      <c r="D10">
-        <v>113</v>
-      </c>
       <c r="E10">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11">
         <v>60</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>83</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>72</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12">
         <v>62</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>102</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
       <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
         <v>32</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>156.77000000000001</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1">
         <v>31</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>61</v>
       </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
       <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
         <v>32</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>156.77000000000001</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="1">
-        <v>0</v>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
         <v>30</v>
       </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
       <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
         <v>32</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>156.77000000000001</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="1">
-        <v>0</v>
+      <c r="C15" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
         <v>30</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <v>33</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>63</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>156.77000000000001</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="1">
+        <v>-120</v>
+      </c>
+      <c r="E16" s="1">
+        <v>120</v>
+      </c>
+      <c r="F16" s="1">
+        <v>-110</v>
+      </c>
+      <c r="G16" s="1">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="1">
+        <v>-120</v>
+      </c>
+      <c r="E17" s="1">
+        <v>120</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>-10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new script to plot both sections on a single plot
</commit_message>
<xml_diff>
--- a/data/sampling/metadata.xlsx
+++ b/data/sampling/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Liam/Desktop/UW/ECM/alhic1901_deep_layering/github/data/sampling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E58CD59-DEA3-D749-BB0C-8B178A712BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354E1BC5-BF7C-2349-BFAE-2A63B29CDCD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="760" windowWidth="29220" windowHeight="18880" xr2:uid="{A8C00553-77EA-744E-A26E-6C00C0051891}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
   <si>
     <t>section</t>
   </si>
@@ -74,73 +74,76 @@
     <t>stick2</t>
   </si>
   <si>
+    <t>l_iso</t>
+  </si>
+  <si>
+    <t>r_iso</t>
+  </si>
+  <si>
+    <t>c_iso</t>
+  </si>
+  <si>
+    <t>stick3</t>
+  </si>
+  <si>
+    <t>stick1</t>
+  </si>
+  <si>
+    <t>offset</t>
+  </si>
+  <si>
+    <t>section_top_depth</t>
+  </si>
+  <si>
+    <t>co2</t>
+  </si>
+  <si>
+    <t>meas_type</t>
+  </si>
+  <si>
+    <t>IC / CC</t>
+  </si>
+  <si>
+    <t>ICMPS</t>
+  </si>
+  <si>
+    <t>CO$_2$</t>
+  </si>
+  <si>
+    <t>CH$_4$</t>
+  </si>
+  <si>
+    <t>ISO</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>thin_section_vert</t>
+  </si>
+  <si>
+    <t>PP</t>
+  </si>
+  <si>
+    <t>ch4</t>
+  </si>
+  <si>
+    <t>default_color</t>
+  </si>
+  <si>
+    <t>rch4</t>
+  </si>
+  <si>
     <t>lco2</t>
-  </si>
-  <si>
-    <t>rch4</t>
-  </si>
-  <si>
-    <t>l_iso</t>
-  </si>
-  <si>
-    <t>r_iso</t>
-  </si>
-  <si>
-    <t>c_iso</t>
-  </si>
-  <si>
-    <t>stick3</t>
-  </si>
-  <si>
-    <t>stick1</t>
-  </si>
-  <si>
-    <t>offset</t>
-  </si>
-  <si>
-    <t>section_top_depth</t>
-  </si>
-  <si>
-    <t>co2</t>
-  </si>
-  <si>
-    <t>meas_type</t>
-  </si>
-  <si>
-    <t>IC / CC</t>
-  </si>
-  <si>
-    <t>ICMPS</t>
-  </si>
-  <si>
-    <t>CO$_2$</t>
-  </si>
-  <si>
-    <t>CH$_4$</t>
-  </si>
-  <si>
-    <t>ISO</t>
-  </si>
-  <si>
-    <t>IC</t>
-  </si>
-  <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>ar</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>thin_section_vert</t>
-  </si>
-  <si>
-    <t>PP</t>
-  </si>
-  <si>
-    <t>ch4</t>
   </si>
 </sst>
 </file>
@@ -519,15 +522,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD79FB1-660A-A74C-AF5D-70A1289F30BA}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -535,7 +541,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -550,13 +556,16 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -564,7 +573,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1">
         <v>-110</v>
@@ -578,8 +587,11 @@
       <c r="G2" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -587,7 +599,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1">
         <v>50</v>
@@ -601,8 +613,11 @@
       <c r="G3" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -610,7 +625,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1">
         <v>80</v>
@@ -624,16 +639,19 @@
       <c r="G4" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5">
         <v>-75</v>
@@ -647,16 +665,19 @@
       <c r="G5">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -670,16 +691,19 @@
       <c r="G6">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>-15</v>
@@ -693,16 +717,19 @@
       <c r="G7">
         <v>-120</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8">
         <v>-110</v>
@@ -716,16 +743,19 @@
       <c r="G8">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9">
         <v>120</v>
@@ -739,16 +769,19 @@
       <c r="G9">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10">
         <v>103</v>
@@ -762,16 +795,19 @@
       <c r="G10">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D11">
         <v>60</v>
@@ -785,16 +821,19 @@
       <c r="G11">
         <v>92</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12">
         <v>62</v>
@@ -814,8 +853,11 @@
       <c r="I12">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -843,16 +885,19 @@
       <c r="I13">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -872,16 +917,19 @@
       <c r="I14">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -901,16 +949,19 @@
       <c r="I15">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D16" s="1">
         <v>-120</v>
@@ -924,16 +975,19 @@
       <c r="G16" s="1">
         <v>-10</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D17" s="1">
         <v>-120</v>
@@ -947,16 +1001,19 @@
       <c r="G17" s="1">
         <v>-10</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D18" s="1">
         <v>30</v>
@@ -975,6 +1032,9 @@
       </c>
       <c r="I18">
         <v>24</v>
+      </c>
+      <c r="J18" s="1">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>